<commit_message>
agregado de notas de 4b, 6a,  7B
</commit_message>
<xml_diff>
--- a/inasistencias-5a-Electornica/alumnos-5a-Electronica.xlsx
+++ b/inasistencias-5a-Electornica/alumnos-5a-Electronica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="asistencia" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,7 @@
     <sheet name="positivos" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="5-parDarlington" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Evaluacion" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Recuperacoin" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="554">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -1682,6 +1683,18 @@
   </si>
   <si>
     <t xml:space="preserve">51 minutos 29 segundos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Act fij polariz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2- par darlington</t>
   </si>
 </sst>
 </file>
@@ -1912,10 +1925,10 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
@@ -3055,7 +3068,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.55"/>
@@ -3366,7 +3379,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
@@ -3928,7 +3941,7 @@
       <selection pane="topLeft" activeCell="I51" activeCellId="0" sqref="I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="21.34"/>
@@ -4912,7 +4925,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.33"/>
@@ -5372,6 +5385,59 @@
         <v>549</v>
       </c>
       <c r="F23" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>552</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -5393,11 +5459,11 @@
   </sheetPr>
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
@@ -6630,7 +6696,7 @@
       <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.64"/>
@@ -7748,7 +7814,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.2"/>
@@ -7886,7 +7952,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.64"/>
@@ -8650,7 +8716,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>
@@ -9091,7 +9157,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
@@ -10211,7 +10277,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.55"/>
@@ -10536,7 +10602,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>

</xml_diff>

<commit_message>
actualizacion de listados y agregado de imagenes de grupos para 6to
</commit_message>
<xml_diff>
--- a/inasistencias-5a-Electornica/alumnos-5a-Electronica.xlsx
+++ b/inasistencias-5a-Electornica/alumnos-5a-Electronica.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="558">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -1985,13 +1985,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R25" activeCellId="0" sqref="R25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S25" activeCellId="0" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
@@ -2076,6 +2076,9 @@
       <c r="R2" s="2" t="n">
         <v>45903</v>
       </c>
+      <c r="S2" s="2" t="n">
+        <v>45910</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -2131,6 +2134,9 @@
       <c r="R3" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S3" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -2186,6 +2192,9 @@
       <c r="R4" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S4" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -2241,6 +2250,9 @@
       <c r="R5" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S5" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -2296,6 +2308,9 @@
       <c r="R6" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S6" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -2351,6 +2366,9 @@
       <c r="R7" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S7" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -2406,6 +2424,9 @@
       <c r="R8" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S8" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -2461,6 +2482,9 @@
       <c r="R9" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S9" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -2514,6 +2538,9 @@
         <v>17</v>
       </c>
       <c r="R10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2571,6 +2598,9 @@
       <c r="R11" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S11" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -2624,6 +2654,9 @@
         <v>10</v>
       </c>
       <c r="R12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2681,6 +2714,9 @@
       <c r="R13" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S13" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -2736,6 +2772,9 @@
       <c r="R14" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S14" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -2791,6 +2830,9 @@
       <c r="R15" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S15" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -2846,6 +2888,9 @@
       <c r="R16" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="S16" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -2901,6 +2946,9 @@
       <c r="R17" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S17" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -2956,6 +3004,9 @@
       <c r="R18" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S18" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -3011,6 +3062,9 @@
       <c r="R19" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S19" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -3066,6 +3120,9 @@
       <c r="R20" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S20" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -3124,6 +3181,9 @@
       <c r="R21" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="S21" s="0" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -3179,6 +3239,9 @@
       <c r="R22" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S22" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -3234,6 +3297,9 @@
       <c r="R23" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="S23" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -3287,6 +3353,9 @@
         <v>10</v>
       </c>
       <c r="R24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S24" s="0" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3334,6 +3403,10 @@
       <c r="R25" s="0" t="n">
         <f aca="false">COUNTIF(R3:R24,"P")</f>
         <v>20</v>
+      </c>
+      <c r="S25" s="0" t="n">
+        <f aca="false">COUNTIF(S3:S24,"P")</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3355,10 +3428,10 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="R25 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="S25 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.55"/>
@@ -3666,10 +3739,10 @@
   <dimension ref="A1:AD23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="R25 J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="S25 J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
@@ -4228,10 +4301,10 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I51" activeCellId="1" sqref="R25 I51"/>
+      <selection pane="topLeft" activeCell="I51" activeCellId="1" sqref="S25 I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="21.34"/>
@@ -5212,10 +5285,10 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="R25 F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="S25 F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.33"/>
@@ -5697,10 +5770,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="R25 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="S25 C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5750,10 +5823,10 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O14" activeCellId="1" sqref="R25 O14"/>
+      <selection pane="topLeft" activeCell="O14" activeCellId="1" sqref="S25 O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
@@ -7092,10 +7165,10 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="1" sqref="R25 I29"/>
+      <selection pane="topLeft" activeCell="I29" activeCellId="1" sqref="S25 I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.64"/>
@@ -8210,10 +8283,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="R25 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="S25 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.2"/>
@@ -8348,10 +8421,10 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="R25 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="S25 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.64"/>
@@ -9112,10 +9185,10 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="R25 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="S25 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>
@@ -9553,10 +9626,10 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="R25 G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="S25 G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
@@ -10673,10 +10746,10 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="R25 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="S25 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.55"/>
@@ -10998,10 +11071,10 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="R25 F4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="S25 F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>

</xml_diff>